<commit_message>
Added excel support and working on import code. Set project to console application until we're ready to get the GUI working. Moved generic methods to Util.cs.
</commit_message>
<xml_diff>
--- a/Format for Hydro$ense Python Solver.xlsx
+++ b/Format for Hydro$ense Python Solver.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="12435" windowHeight="9465"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="12435" windowHeight="9465" tabRatio="719"/>
   </bookViews>
   <sheets>
     <sheet name="Problem Setup" sheetId="1" r:id="rId1"/>
     <sheet name="Problem Solution" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Supply Curves" sheetId="4" r:id="rId3"/>
+    <sheet name="Demand Curves" sheetId="5" r:id="rId4"/>
+    <sheet name="Transportation Costs" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -5398,18 +5400,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5715,8 +5717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5728,15 +5730,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -5744,114 +5746,114 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
@@ -7001,26 +7003,26 @@
       </c>
     </row>
     <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="16" t="s">
+      <c r="A79" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
     </row>
     <row r="80" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C80" s="17"/>
-      <c r="D80" s="17"/>
-      <c r="E80" s="17"/>
-      <c r="F80" s="17"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
-      <c r="J80" s="17"/>
-      <c r="K80" s="17"/>
-      <c r="L80" s="17"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+      <c r="K80" s="19"/>
+      <c r="L80" s="19"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
@@ -8422,12 +8424,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:G7"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="B80:L80"/>
     <mergeCell ref="A11:G11"/>
@@ -8435,6 +8431,12 @@
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8524,12 +8526,711 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>IF(ISNUMBER('Problem Setup'!B41),'Problem Setup'!B41,"")</f>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <f>IF(ISNUMBER('Problem Setup'!C41),'Problem Setup'!C41,"")</f>
+        <v>2000</v>
+      </c>
+      <c r="C1">
+        <f>IF(ISNUMBER('Problem Setup'!D41),'Problem Setup'!D41,"")</f>
+        <v>4000</v>
+      </c>
+      <c r="D1">
+        <f>IF(ISNUMBER('Problem Setup'!E41),'Problem Setup'!E41,"")</f>
+        <v>5000</v>
+      </c>
+      <c r="E1">
+        <f>IF(ISNUMBER('Problem Setup'!F41),'Problem Setup'!F41,"")</f>
+        <v>7500</v>
+      </c>
+      <c r="F1">
+        <f>IF(ISNUMBER('Problem Setup'!G41),'Problem Setup'!G41,"")</f>
+        <v>10000</v>
+      </c>
+      <c r="G1">
+        <f>IF(ISNUMBER('Problem Setup'!H41),'Problem Setup'!H41,"")</f>
+        <v>20000</v>
+      </c>
+      <c r="H1">
+        <f>IF(ISNUMBER('Problem Setup'!I41),'Problem Setup'!I41,"")</f>
+        <v>30000</v>
+      </c>
+      <c r="I1">
+        <f>IF(ISNUMBER('Problem Setup'!J41),'Problem Setup'!J41,"")</f>
+        <v>50000</v>
+      </c>
+      <c r="J1">
+        <f>IF(ISNUMBER('Problem Setup'!K41),'Problem Setup'!K41,"")</f>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>IF(ISNUMBER('Problem Setup'!B42),'Problem Setup'!B42,"")</f>
+        <v>3</v>
+      </c>
+      <c r="B2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!C42),'Problem Setup'!C42,"")</f>
+        <v>3.0606040200802673</v>
+      </c>
+      <c r="C2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!D42),'Problem Setup'!D42,"")</f>
+        <v>3.1224323225771649</v>
+      </c>
+      <c r="D2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!E42),'Problem Setup'!E42,"")</f>
+        <v>3.1538132891280721</v>
+      </c>
+      <c r="E2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!F42),'Problem Setup'!F42,"")</f>
+        <v>3.2336524526538946</v>
+      </c>
+      <c r="F2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!G42),'Problem Setup'!G42,"")</f>
+        <v>3.3155127542269431</v>
+      </c>
+      <c r="G2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!H42),'Problem Setup'!H42,"")</f>
+        <v>3.6642082744805098</v>
+      </c>
+      <c r="H2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!I42),'Problem Setup'!I42,"")</f>
+        <v>4.0495764227280091</v>
+      </c>
+      <c r="I2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!J42),'Problem Setup'!J42,"")</f>
+        <v>4.9461638121003846</v>
+      </c>
+      <c r="J2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!K42),'Problem Setup'!K42,"")</f>
+        <v>5.7466224870416891</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>IF(ISNUMBER('Problem Setup'!B43),'Problem Setup'!B43,"")</f>
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>IF(ISNUMBER('Problem Setup'!C43),'Problem Setup'!C43,"")</f>
+        <v>1000</v>
+      </c>
+      <c r="C3">
+        <f>IF(ISNUMBER('Problem Setup'!D43),'Problem Setup'!D43,"")</f>
+        <v>2500</v>
+      </c>
+      <c r="D3">
+        <f>IF(ISNUMBER('Problem Setup'!E43),'Problem Setup'!E43,"")</f>
+        <v>5000</v>
+      </c>
+      <c r="E3">
+        <f>IF(ISNUMBER('Problem Setup'!F43),'Problem Setup'!F43,"")</f>
+        <v>8000</v>
+      </c>
+      <c r="F3">
+        <f>IF(ISNUMBER('Problem Setup'!G43),'Problem Setup'!G43,"")</f>
+        <v>10000</v>
+      </c>
+      <c r="G3">
+        <f>IF(ISNUMBER('Problem Setup'!H43),'Problem Setup'!H43,"")</f>
+        <v>15000</v>
+      </c>
+      <c r="H3">
+        <f>IF(ISNUMBER('Problem Setup'!I43),'Problem Setup'!I43,"")</f>
+        <v>25000</v>
+      </c>
+      <c r="I3" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!J43),'Problem Setup'!J43,"")</f>
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K43),'Problem Setup'!K43,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>IF(ISNUMBER('Problem Setup'!B44),'Problem Setup'!B44,"")</f>
+        <v>1.5</v>
+      </c>
+      <c r="B4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!C44),'Problem Setup'!C44,"")</f>
+        <v>1.5456818009302755</v>
+      </c>
+      <c r="C4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!D44),'Problem Setup'!D44,"")</f>
+        <v>1.6168262263269473</v>
+      </c>
+      <c r="D4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!E44),'Problem Setup'!E44,"")</f>
+        <v>1.7427513640924246</v>
+      </c>
+      <c r="E4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!F44),'Problem Setup'!F44,"")</f>
+        <v>1.9068737254821071</v>
+      </c>
+      <c r="F4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!G44),'Problem Setup'!G44,"")</f>
+        <v>2.0247882113640046</v>
+      </c>
+      <c r="G4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!H44),'Problem Setup'!H44,"")</f>
+        <v>2.3524682782352535</v>
+      </c>
+      <c r="H4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!I44),'Problem Setup'!I44,"")</f>
+        <v>3.1755000249190122</v>
+      </c>
+      <c r="I4" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!J44),'Problem Setup'!J44,"")</f>
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K44),'Problem Setup'!K44,"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>IF(ISNUMBER('Problem Setup'!B46),'Problem Setup'!B46,"")</f>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <f>IF(ISNUMBER('Problem Setup'!C46),'Problem Setup'!C46,"")</f>
+        <v>2000</v>
+      </c>
+      <c r="C1">
+        <f>IF(ISNUMBER('Problem Setup'!D46),'Problem Setup'!D46,"")</f>
+        <v>4000</v>
+      </c>
+      <c r="D1">
+        <f>IF(ISNUMBER('Problem Setup'!E46),'Problem Setup'!E46,"")</f>
+        <v>7500</v>
+      </c>
+      <c r="E1">
+        <f>IF(ISNUMBER('Problem Setup'!F46),'Problem Setup'!F46,"")</f>
+        <v>10000</v>
+      </c>
+      <c r="F1">
+        <f>IF(ISNUMBER('Problem Setup'!G46),'Problem Setup'!G46,"")</f>
+        <v>15000</v>
+      </c>
+      <c r="G1">
+        <f>IF(ISNUMBER('Problem Setup'!H46),'Problem Setup'!H46,"")</f>
+        <v>20000</v>
+      </c>
+      <c r="H1">
+        <f>IF(ISNUMBER('Problem Setup'!I46),'Problem Setup'!I46,"")</f>
+        <v>30000</v>
+      </c>
+      <c r="I1">
+        <f>IF(ISNUMBER('Problem Setup'!J46),'Problem Setup'!J46,"")</f>
+        <v>40000</v>
+      </c>
+      <c r="J1" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K46),'Problem Setup'!K46,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>IF(ISNUMBER('Problem Setup'!B47),'Problem Setup'!B47,"")</f>
+        <v>15</v>
+      </c>
+      <c r="B2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!C47),'Problem Setup'!C47,"")</f>
+        <v>12.78215683449317</v>
+      </c>
+      <c r="C2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!D47),'Problem Setup'!D47,"")</f>
+        <v>10.892235556105364</v>
+      </c>
+      <c r="D2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!E47),'Problem Setup'!E47,"")</f>
+        <v>8.2321745414103962</v>
+      </c>
+      <c r="E2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!F47),'Problem Setup'!F47,"")</f>
+        <v>6.7399344617583239</v>
+      </c>
+      <c r="F2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!G47),'Problem Setup'!G47,"")</f>
+        <v>4.5179131786830302</v>
+      </c>
+      <c r="G2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!H47),'Problem Setup'!H47,"")</f>
+        <v>3.0284477699198309</v>
+      </c>
+      <c r="H2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!I47),'Problem Setup'!I47,"")</f>
+        <v>1.3607692993411871</v>
+      </c>
+      <c r="I2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!J47),'Problem Setup'!J47,"")</f>
+        <v>0.61143305967549322</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K47),'Problem Setup'!K47,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>IF(ISNUMBER('Problem Setup'!B48),'Problem Setup'!B48,"")</f>
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>IF(ISNUMBER('Problem Setup'!C48),'Problem Setup'!C48,"")</f>
+        <v>3000</v>
+      </c>
+      <c r="C3">
+        <f>IF(ISNUMBER('Problem Setup'!D48),'Problem Setup'!D48,"")</f>
+        <v>7500</v>
+      </c>
+      <c r="D3">
+        <f>IF(ISNUMBER('Problem Setup'!E48),'Problem Setup'!E48,"")</f>
+        <v>12500</v>
+      </c>
+      <c r="E3">
+        <f>IF(ISNUMBER('Problem Setup'!F48),'Problem Setup'!F48,"")</f>
+        <v>20000</v>
+      </c>
+      <c r="F3">
+        <f>IF(ISNUMBER('Problem Setup'!G48),'Problem Setup'!G48,"")</f>
+        <v>30000</v>
+      </c>
+      <c r="G3" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!H48),'Problem Setup'!H48,"")</f>
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!I48),'Problem Setup'!I48,"")</f>
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!J48),'Problem Setup'!J48,"")</f>
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K48),'Problem Setup'!K48,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>IF(ISNUMBER('Problem Setup'!B49),'Problem Setup'!B49,"")</f>
+        <v>10</v>
+      </c>
+      <c r="B4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!C49),'Problem Setup'!C49,"")</f>
+        <v>8.6070797642505781</v>
+      </c>
+      <c r="C4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!D49),'Problem Setup'!D49,"")</f>
+        <v>6.8728927879097226</v>
+      </c>
+      <c r="D4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!E49),'Problem Setup'!E49,"")</f>
+        <v>5.3526142851899028</v>
+      </c>
+      <c r="E4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!F49),'Problem Setup'!F49,"")</f>
+        <v>3.6787944117144233</v>
+      </c>
+      <c r="F4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!G49),'Problem Setup'!G49,"")</f>
+        <v>2.2313016014842981</v>
+      </c>
+      <c r="G4" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!H49),'Problem Setup'!H49,"")</f>
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!I49),'Problem Setup'!I49,"")</f>
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!J49),'Problem Setup'!J49,"")</f>
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K49),'Problem Setup'!K49,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>IF(ISNUMBER('Problem Setup'!B50),'Problem Setup'!B50,"")</f>
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <f>IF(ISNUMBER('Problem Setup'!C50),'Problem Setup'!C50,"")</f>
+        <v>2500</v>
+      </c>
+      <c r="C5">
+        <f>IF(ISNUMBER('Problem Setup'!D50),'Problem Setup'!D50,"")</f>
+        <v>5000</v>
+      </c>
+      <c r="D5">
+        <f>IF(ISNUMBER('Problem Setup'!E50),'Problem Setup'!E50,"")</f>
+        <v>10000</v>
+      </c>
+      <c r="E5">
+        <f>IF(ISNUMBER('Problem Setup'!F50),'Problem Setup'!F50,"")</f>
+        <v>15000</v>
+      </c>
+      <c r="F5">
+        <f>IF(ISNUMBER('Problem Setup'!G50),'Problem Setup'!G50,"")</f>
+        <v>25000</v>
+      </c>
+      <c r="G5">
+        <f>IF(ISNUMBER('Problem Setup'!H50),'Problem Setup'!H50,"")</f>
+        <v>35000</v>
+      </c>
+      <c r="H5" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!I50),'Problem Setup'!I50,"")</f>
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!J50),'Problem Setup'!J50,"")</f>
+        <v/>
+      </c>
+      <c r="J5" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K50),'Problem Setup'!K50,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>IF(ISNUMBER('Problem Setup'!B51),'Problem Setup'!B51,"")</f>
+        <v>25</v>
+      </c>
+      <c r="B6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!C51),'Problem Setup'!C51,"")</f>
+        <v>19.470019576785123</v>
+      </c>
+      <c r="C6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!D51),'Problem Setup'!D51,"")</f>
+        <v>15.163266492815836</v>
+      </c>
+      <c r="D6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!E51),'Problem Setup'!E51,"")</f>
+        <v>9.1969860292860588</v>
+      </c>
+      <c r="E6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!F51),'Problem Setup'!F51,"")</f>
+        <v>5.5782540037107458</v>
+      </c>
+      <c r="F6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!G51),'Problem Setup'!G51,"")</f>
+        <v>2.05212496559747</v>
+      </c>
+      <c r="G6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!H51),'Problem Setup'!H51,"")</f>
+        <v>0.75493458555796256</v>
+      </c>
+      <c r="H6" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!I51),'Problem Setup'!I51,"")</f>
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!J51),'Problem Setup'!J51,"")</f>
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K51),'Problem Setup'!K51,"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>IF(ISNUMBER('Problem Setup'!B46),'Problem Setup'!B46,"")</f>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <f>IF(ISNUMBER('Problem Setup'!C46),'Problem Setup'!C46,"")</f>
+        <v>2000</v>
+      </c>
+      <c r="C1">
+        <f>IF(ISNUMBER('Problem Setup'!D46),'Problem Setup'!D46,"")</f>
+        <v>4000</v>
+      </c>
+      <c r="D1">
+        <f>IF(ISNUMBER('Problem Setup'!E46),'Problem Setup'!E46,"")</f>
+        <v>7500</v>
+      </c>
+      <c r="E1">
+        <f>IF(ISNUMBER('Problem Setup'!F46),'Problem Setup'!F46,"")</f>
+        <v>10000</v>
+      </c>
+      <c r="F1">
+        <f>IF(ISNUMBER('Problem Setup'!G46),'Problem Setup'!G46,"")</f>
+        <v>15000</v>
+      </c>
+      <c r="G1">
+        <f>IF(ISNUMBER('Problem Setup'!H46),'Problem Setup'!H46,"")</f>
+        <v>20000</v>
+      </c>
+      <c r="H1">
+        <f>IF(ISNUMBER('Problem Setup'!I46),'Problem Setup'!I46,"")</f>
+        <v>30000</v>
+      </c>
+      <c r="I1">
+        <f>IF(ISNUMBER('Problem Setup'!J46),'Problem Setup'!J46,"")</f>
+        <v>40000</v>
+      </c>
+      <c r="J1" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K46),'Problem Setup'!K46,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>IF(ISNUMBER('Problem Setup'!B47),'Problem Setup'!B47,"")</f>
+        <v>15</v>
+      </c>
+      <c r="B2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!C47),'Problem Setup'!C47,"")</f>
+        <v>12.78215683449317</v>
+      </c>
+      <c r="C2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!D47),'Problem Setup'!D47,"")</f>
+        <v>10.892235556105364</v>
+      </c>
+      <c r="D2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!E47),'Problem Setup'!E47,"")</f>
+        <v>8.2321745414103962</v>
+      </c>
+      <c r="E2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!F47),'Problem Setup'!F47,"")</f>
+        <v>6.7399344617583239</v>
+      </c>
+      <c r="F2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!G47),'Problem Setup'!G47,"")</f>
+        <v>4.5179131786830302</v>
+      </c>
+      <c r="G2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!H47),'Problem Setup'!H47,"")</f>
+        <v>3.0284477699198309</v>
+      </c>
+      <c r="H2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!I47),'Problem Setup'!I47,"")</f>
+        <v>1.3607692993411871</v>
+      </c>
+      <c r="I2" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!J47),'Problem Setup'!J47,"")</f>
+        <v>0.61143305967549322</v>
+      </c>
+      <c r="J2" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K47),'Problem Setup'!K47,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>IF(ISNUMBER('Problem Setup'!B48),'Problem Setup'!B48,"")</f>
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>IF(ISNUMBER('Problem Setup'!C48),'Problem Setup'!C48,"")</f>
+        <v>3000</v>
+      </c>
+      <c r="C3">
+        <f>IF(ISNUMBER('Problem Setup'!D48),'Problem Setup'!D48,"")</f>
+        <v>7500</v>
+      </c>
+      <c r="D3">
+        <f>IF(ISNUMBER('Problem Setup'!E48),'Problem Setup'!E48,"")</f>
+        <v>12500</v>
+      </c>
+      <c r="E3">
+        <f>IF(ISNUMBER('Problem Setup'!F48),'Problem Setup'!F48,"")</f>
+        <v>20000</v>
+      </c>
+      <c r="F3">
+        <f>IF(ISNUMBER('Problem Setup'!G48),'Problem Setup'!G48,"")</f>
+        <v>30000</v>
+      </c>
+      <c r="G3" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!H48),'Problem Setup'!H48,"")</f>
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!I48),'Problem Setup'!I48,"")</f>
+        <v/>
+      </c>
+      <c r="I3" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!J48),'Problem Setup'!J48,"")</f>
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K48),'Problem Setup'!K48,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>IF(ISNUMBER('Problem Setup'!B49),'Problem Setup'!B49,"")</f>
+        <v>10</v>
+      </c>
+      <c r="B4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!C49),'Problem Setup'!C49,"")</f>
+        <v>8.6070797642505781</v>
+      </c>
+      <c r="C4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!D49),'Problem Setup'!D49,"")</f>
+        <v>6.8728927879097226</v>
+      </c>
+      <c r="D4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!E49),'Problem Setup'!E49,"")</f>
+        <v>5.3526142851899028</v>
+      </c>
+      <c r="E4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!F49),'Problem Setup'!F49,"")</f>
+        <v>3.6787944117144233</v>
+      </c>
+      <c r="F4" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!G49),'Problem Setup'!G49,"")</f>
+        <v>2.2313016014842981</v>
+      </c>
+      <c r="G4" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!H49),'Problem Setup'!H49,"")</f>
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!I49),'Problem Setup'!I49,"")</f>
+        <v/>
+      </c>
+      <c r="I4" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!J49),'Problem Setup'!J49,"")</f>
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K49),'Problem Setup'!K49,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>IF(ISNUMBER('Problem Setup'!B50),'Problem Setup'!B50,"")</f>
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <f>IF(ISNUMBER('Problem Setup'!C50),'Problem Setup'!C50,"")</f>
+        <v>2500</v>
+      </c>
+      <c r="C5">
+        <f>IF(ISNUMBER('Problem Setup'!D50),'Problem Setup'!D50,"")</f>
+        <v>5000</v>
+      </c>
+      <c r="D5">
+        <f>IF(ISNUMBER('Problem Setup'!E50),'Problem Setup'!E50,"")</f>
+        <v>10000</v>
+      </c>
+      <c r="E5">
+        <f>IF(ISNUMBER('Problem Setup'!F50),'Problem Setup'!F50,"")</f>
+        <v>15000</v>
+      </c>
+      <c r="F5">
+        <f>IF(ISNUMBER('Problem Setup'!G50),'Problem Setup'!G50,"")</f>
+        <v>25000</v>
+      </c>
+      <c r="G5">
+        <f>IF(ISNUMBER('Problem Setup'!H50),'Problem Setup'!H50,"")</f>
+        <v>35000</v>
+      </c>
+      <c r="H5" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!I50),'Problem Setup'!I50,"")</f>
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!J50),'Problem Setup'!J50,"")</f>
+        <v/>
+      </c>
+      <c r="J5" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K50),'Problem Setup'!K50,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>IF(ISNUMBER('Problem Setup'!B51),'Problem Setup'!B51,"")</f>
+        <v>25</v>
+      </c>
+      <c r="B6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!C51),'Problem Setup'!C51,"")</f>
+        <v>19.470019576785123</v>
+      </c>
+      <c r="C6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!D51),'Problem Setup'!D51,"")</f>
+        <v>15.163266492815836</v>
+      </c>
+      <c r="D6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!E51),'Problem Setup'!E51,"")</f>
+        <v>9.1969860292860588</v>
+      </c>
+      <c r="E6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!F51),'Problem Setup'!F51,"")</f>
+        <v>5.5782540037107458</v>
+      </c>
+      <c r="F6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!G51),'Problem Setup'!G51,"")</f>
+        <v>2.05212496559747</v>
+      </c>
+      <c r="G6" s="6">
+        <f>IF(ISNUMBER('Problem Setup'!H51),'Problem Setup'!H51,"")</f>
+        <v>0.75493458555796256</v>
+      </c>
+      <c r="H6" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!I51),'Problem Setup'!I51,"")</f>
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!J51),'Problem Setup'!J51,"")</f>
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <f>IF(ISNUMBER('Problem Setup'!K51),'Problem Setup'!K51,"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Import from Excel complete. I get the same result with hard-coded or Excel import.
</commit_message>
<xml_diff>
--- a/Format for Hydro$ense Python Solver.xlsx
+++ b/Format for Hydro$ense Python Solver.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="12435" windowHeight="9465" tabRatio="719"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="12435" windowHeight="9465" tabRatio="827" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Problem Setup" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,8 @@
     <sheet name="Supply Curves" sheetId="4" r:id="rId3"/>
     <sheet name="Demand Curves" sheetId="5" r:id="rId4"/>
     <sheet name="Transportation Costs" sheetId="7" r:id="rId5"/>
+    <sheet name="Transportation Losses" sheetId="8" r:id="rId6"/>
+    <sheet name="Initial Guess" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -5400,18 +5402,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5717,7 +5719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A106" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
@@ -5730,15 +5732,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -5746,114 +5748,114 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
     </row>
     <row r="6" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
     </row>
     <row r="7" spans="1:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
     </row>
     <row r="10" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
     </row>
     <row r="11" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
@@ -7003,26 +7005,26 @@
       </c>
     </row>
     <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
     </row>
     <row r="80" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="19" t="s">
+      <c r="B80" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="C80" s="19"/>
-      <c r="D80" s="19"/>
-      <c r="E80" s="19"/>
-      <c r="F80" s="19"/>
-      <c r="G80" s="19"/>
-      <c r="H80" s="19"/>
-      <c r="I80" s="19"/>
-      <c r="J80" s="19"/>
-      <c r="K80" s="19"/>
-      <c r="L80" s="19"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
+      <c r="J80" s="17"/>
+      <c r="K80" s="17"/>
+      <c r="L80" s="17"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
@@ -8424,6 +8426,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="B80:L80"/>
     <mergeCell ref="A11:G11"/>
@@ -8431,12 +8439,6 @@
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8528,175 +8530,175 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
-        <f>IF(ISNUMBER('Problem Setup'!B41),'Problem Setup'!B41,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!B41),ROUND('Problem Setup'!B41,3),"")</f>
         <v>0</v>
       </c>
       <c r="B1">
-        <f>IF(ISNUMBER('Problem Setup'!C41),'Problem Setup'!C41,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!C41),ROUND('Problem Setup'!C41,3),"")</f>
         <v>2000</v>
       </c>
       <c r="C1">
-        <f>IF(ISNUMBER('Problem Setup'!D41),'Problem Setup'!D41,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!D41),ROUND('Problem Setup'!D41,3),"")</f>
         <v>4000</v>
       </c>
       <c r="D1">
-        <f>IF(ISNUMBER('Problem Setup'!E41),'Problem Setup'!E41,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!E41),ROUND('Problem Setup'!E41,3),"")</f>
         <v>5000</v>
       </c>
       <c r="E1">
-        <f>IF(ISNUMBER('Problem Setup'!F41),'Problem Setup'!F41,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!F41),ROUND('Problem Setup'!F41,3),"")</f>
         <v>7500</v>
       </c>
       <c r="F1">
-        <f>IF(ISNUMBER('Problem Setup'!G41),'Problem Setup'!G41,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!G41),ROUND('Problem Setup'!G41,3),"")</f>
         <v>10000</v>
       </c>
       <c r="G1">
-        <f>IF(ISNUMBER('Problem Setup'!H41),'Problem Setup'!H41,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!H41),ROUND('Problem Setup'!H41,3),"")</f>
         <v>20000</v>
       </c>
       <c r="H1">
-        <f>IF(ISNUMBER('Problem Setup'!I41),'Problem Setup'!I41,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!I41),ROUND('Problem Setup'!I41,3),"")</f>
         <v>30000</v>
       </c>
       <c r="I1">
-        <f>IF(ISNUMBER('Problem Setup'!J41),'Problem Setup'!J41,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!J41),ROUND('Problem Setup'!J41,3),"")</f>
         <v>50000</v>
       </c>
       <c r="J1">
-        <f>IF(ISNUMBER('Problem Setup'!K41),'Problem Setup'!K41,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!K41),ROUND('Problem Setup'!K41,3),"")</f>
         <v>65000</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>IF(ISNUMBER('Problem Setup'!B42),'Problem Setup'!B42,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!B42),ROUND('Problem Setup'!B42,3),"")</f>
         <v>3</v>
       </c>
-      <c r="B2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!C42),'Problem Setup'!C42,"")</f>
-        <v>3.0606040200802673</v>
-      </c>
-      <c r="C2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!D42),'Problem Setup'!D42,"")</f>
-        <v>3.1224323225771649</v>
-      </c>
-      <c r="D2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!E42),'Problem Setup'!E42,"")</f>
-        <v>3.1538132891280721</v>
-      </c>
-      <c r="E2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!F42),'Problem Setup'!F42,"")</f>
-        <v>3.2336524526538946</v>
-      </c>
-      <c r="F2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!G42),'Problem Setup'!G42,"")</f>
-        <v>3.3155127542269431</v>
-      </c>
-      <c r="G2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!H42),'Problem Setup'!H42,"")</f>
-        <v>3.6642082744805098</v>
-      </c>
-      <c r="H2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!I42),'Problem Setup'!I42,"")</f>
-        <v>4.0495764227280091</v>
-      </c>
-      <c r="I2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!J42),'Problem Setup'!J42,"")</f>
-        <v>4.9461638121003846</v>
-      </c>
-      <c r="J2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!K42),'Problem Setup'!K42,"")</f>
-        <v>5.7466224870416891</v>
+      <c r="B2">
+        <f>IF(ISNUMBER('Problem Setup'!C42),ROUND('Problem Setup'!C42,3),"")</f>
+        <v>3.0609999999999999</v>
+      </c>
+      <c r="C2">
+        <f>IF(ISNUMBER('Problem Setup'!D42),ROUND('Problem Setup'!D42,3),"")</f>
+        <v>3.1219999999999999</v>
+      </c>
+      <c r="D2">
+        <f>IF(ISNUMBER('Problem Setup'!E42),ROUND('Problem Setup'!E42,3),"")</f>
+        <v>3.1539999999999999</v>
+      </c>
+      <c r="E2">
+        <f>IF(ISNUMBER('Problem Setup'!F42),ROUND('Problem Setup'!F42,3),"")</f>
+        <v>3.234</v>
+      </c>
+      <c r="F2">
+        <f>IF(ISNUMBER('Problem Setup'!G42),ROUND('Problem Setup'!G42,3),"")</f>
+        <v>3.3159999999999998</v>
+      </c>
+      <c r="G2">
+        <f>IF(ISNUMBER('Problem Setup'!H42),ROUND('Problem Setup'!H42,3),"")</f>
+        <v>3.6640000000000001</v>
+      </c>
+      <c r="H2">
+        <f>IF(ISNUMBER('Problem Setup'!I42),ROUND('Problem Setup'!I42,3),"")</f>
+        <v>4.05</v>
+      </c>
+      <c r="I2">
+        <f>IF(ISNUMBER('Problem Setup'!J42),ROUND('Problem Setup'!J42,3),"")</f>
+        <v>4.9459999999999997</v>
+      </c>
+      <c r="J2">
+        <f>IF(ISNUMBER('Problem Setup'!K42),ROUND('Problem Setup'!K42,3),"")</f>
+        <v>5.7469999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>IF(ISNUMBER('Problem Setup'!B43),'Problem Setup'!B43,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!B43),ROUND('Problem Setup'!B43,3),"")</f>
         <v>0</v>
       </c>
       <c r="B3">
-        <f>IF(ISNUMBER('Problem Setup'!C43),'Problem Setup'!C43,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!C43),ROUND('Problem Setup'!C43,3),"")</f>
         <v>1000</v>
       </c>
       <c r="C3">
-        <f>IF(ISNUMBER('Problem Setup'!D43),'Problem Setup'!D43,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!D43),ROUND('Problem Setup'!D43,3),"")</f>
         <v>2500</v>
       </c>
       <c r="D3">
-        <f>IF(ISNUMBER('Problem Setup'!E43),'Problem Setup'!E43,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!E43),ROUND('Problem Setup'!E43,3),"")</f>
         <v>5000</v>
       </c>
       <c r="E3">
-        <f>IF(ISNUMBER('Problem Setup'!F43),'Problem Setup'!F43,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!F43),ROUND('Problem Setup'!F43,3),"")</f>
         <v>8000</v>
       </c>
       <c r="F3">
-        <f>IF(ISNUMBER('Problem Setup'!G43),'Problem Setup'!G43,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!G43),ROUND('Problem Setup'!G43,3),"")</f>
         <v>10000</v>
       </c>
       <c r="G3">
-        <f>IF(ISNUMBER('Problem Setup'!H43),'Problem Setup'!H43,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!H43),ROUND('Problem Setup'!H43,3),"")</f>
         <v>15000</v>
       </c>
       <c r="H3">
-        <f>IF(ISNUMBER('Problem Setup'!I43),'Problem Setup'!I43,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!I43),ROUND('Problem Setup'!I43,3),"")</f>
         <v>25000</v>
       </c>
       <c r="I3" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!J43),'Problem Setup'!J43,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!J43),ROUND('Problem Setup'!J43,3),"")</f>
         <v/>
       </c>
       <c r="J3" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!K43),'Problem Setup'!K43,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!K43),ROUND('Problem Setup'!K43,3),"")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>IF(ISNUMBER('Problem Setup'!B44),'Problem Setup'!B44,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!B44),ROUND('Problem Setup'!B44,3),"")</f>
         <v>1.5</v>
       </c>
-      <c r="B4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!C44),'Problem Setup'!C44,"")</f>
-        <v>1.5456818009302755</v>
-      </c>
-      <c r="C4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!D44),'Problem Setup'!D44,"")</f>
-        <v>1.6168262263269473</v>
-      </c>
-      <c r="D4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!E44),'Problem Setup'!E44,"")</f>
-        <v>1.7427513640924246</v>
-      </c>
-      <c r="E4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!F44),'Problem Setup'!F44,"")</f>
-        <v>1.9068737254821071</v>
-      </c>
-      <c r="F4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!G44),'Problem Setup'!G44,"")</f>
-        <v>2.0247882113640046</v>
-      </c>
-      <c r="G4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!H44),'Problem Setup'!H44,"")</f>
-        <v>2.3524682782352535</v>
-      </c>
-      <c r="H4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!I44),'Problem Setup'!I44,"")</f>
-        <v>3.1755000249190122</v>
+      <c r="B4">
+        <f>IF(ISNUMBER('Problem Setup'!C44),ROUND('Problem Setup'!C44,3),"")</f>
+        <v>1.546</v>
+      </c>
+      <c r="C4">
+        <f>IF(ISNUMBER('Problem Setup'!D44),ROUND('Problem Setup'!D44,3),"")</f>
+        <v>1.617</v>
+      </c>
+      <c r="D4">
+        <f>IF(ISNUMBER('Problem Setup'!E44),ROUND('Problem Setup'!E44,3),"")</f>
+        <v>1.7430000000000001</v>
+      </c>
+      <c r="E4">
+        <f>IF(ISNUMBER('Problem Setup'!F44),ROUND('Problem Setup'!F44,3),"")</f>
+        <v>1.907</v>
+      </c>
+      <c r="F4">
+        <f>IF(ISNUMBER('Problem Setup'!G44),ROUND('Problem Setup'!G44,3),"")</f>
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="G4">
+        <f>IF(ISNUMBER('Problem Setup'!H44),ROUND('Problem Setup'!H44,3),"")</f>
+        <v>2.3519999999999999</v>
+      </c>
+      <c r="H4">
+        <f>IF(ISNUMBER('Problem Setup'!I44),ROUND('Problem Setup'!I44,3),"")</f>
+        <v>3.1760000000000002</v>
       </c>
       <c r="I4" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!J44),'Problem Setup'!J44,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!J44),ROUND('Problem Setup'!J44,3),"")</f>
         <v/>
       </c>
       <c r="J4" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!K44),'Problem Setup'!K44,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!K44),ROUND('Problem Setup'!K44,3),"")</f>
         <v/>
       </c>
     </row>
@@ -8715,39 +8717,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1">
-        <f>IF(ISNUMBER('Problem Setup'!B46),'Problem Setup'!B46,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!B46),ROUND('Problem Setup'!B46,3),"")</f>
         <v>0</v>
       </c>
       <c r="B1">
-        <f>IF(ISNUMBER('Problem Setup'!C46),'Problem Setup'!C46,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!C46),ROUND('Problem Setup'!C46,3),"")</f>
         <v>2000</v>
       </c>
       <c r="C1">
-        <f>IF(ISNUMBER('Problem Setup'!D46),'Problem Setup'!D46,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!D46),ROUND('Problem Setup'!D46,3),"")</f>
         <v>4000</v>
       </c>
       <c r="D1">
-        <f>IF(ISNUMBER('Problem Setup'!E46),'Problem Setup'!E46,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!E46),ROUND('Problem Setup'!E46,3),"")</f>
         <v>7500</v>
       </c>
       <c r="E1">
-        <f>IF(ISNUMBER('Problem Setup'!F46),'Problem Setup'!F46,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!F46),ROUND('Problem Setup'!F46,3),"")</f>
         <v>10000</v>
       </c>
       <c r="F1">
-        <f>IF(ISNUMBER('Problem Setup'!G46),'Problem Setup'!G46,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!G46),ROUND('Problem Setup'!G46,3),"")</f>
         <v>15000</v>
       </c>
       <c r="G1">
-        <f>IF(ISNUMBER('Problem Setup'!H46),'Problem Setup'!H46,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!H46),ROUND('Problem Setup'!H46,3),"")</f>
         <v>20000</v>
       </c>
       <c r="H1">
-        <f>IF(ISNUMBER('Problem Setup'!I46),'Problem Setup'!I46,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!I46),ROUND('Problem Setup'!I46,3),"")</f>
         <v>30000</v>
       </c>
       <c r="I1">
-        <f>IF(ISNUMBER('Problem Setup'!J46),'Problem Setup'!J46,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!J46),ROUND('Problem Setup'!J46,3),"")</f>
         <v>40000</v>
       </c>
       <c r="J1" t="str">
@@ -8757,40 +8759,40 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>IF(ISNUMBER('Problem Setup'!B47),'Problem Setup'!B47,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!B47),ROUND('Problem Setup'!B47,3),"")</f>
         <v>15</v>
       </c>
-      <c r="B2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!C47),'Problem Setup'!C47,"")</f>
-        <v>12.78215683449317</v>
-      </c>
-      <c r="C2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!D47),'Problem Setup'!D47,"")</f>
-        <v>10.892235556105364</v>
-      </c>
-      <c r="D2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!E47),'Problem Setup'!E47,"")</f>
-        <v>8.2321745414103962</v>
-      </c>
-      <c r="E2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!F47),'Problem Setup'!F47,"")</f>
-        <v>6.7399344617583239</v>
-      </c>
-      <c r="F2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!G47),'Problem Setup'!G47,"")</f>
-        <v>4.5179131786830302</v>
-      </c>
-      <c r="G2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!H47),'Problem Setup'!H47,"")</f>
-        <v>3.0284477699198309</v>
-      </c>
-      <c r="H2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!I47),'Problem Setup'!I47,"")</f>
-        <v>1.3607692993411871</v>
-      </c>
-      <c r="I2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!J47),'Problem Setup'!J47,"")</f>
-        <v>0.61143305967549322</v>
+      <c r="B2">
+        <f>IF(ISNUMBER('Problem Setup'!C47),ROUND('Problem Setup'!C47,3),"")</f>
+        <v>12.782</v>
+      </c>
+      <c r="C2">
+        <f>IF(ISNUMBER('Problem Setup'!D47),ROUND('Problem Setup'!D47,3),"")</f>
+        <v>10.891999999999999</v>
+      </c>
+      <c r="D2">
+        <f>IF(ISNUMBER('Problem Setup'!E47),ROUND('Problem Setup'!E47,3),"")</f>
+        <v>8.2319999999999993</v>
+      </c>
+      <c r="E2">
+        <f>IF(ISNUMBER('Problem Setup'!F47),ROUND('Problem Setup'!F47,3),"")</f>
+        <v>6.74</v>
+      </c>
+      <c r="F2">
+        <f>IF(ISNUMBER('Problem Setup'!G47),ROUND('Problem Setup'!G47,3),"")</f>
+        <v>4.5179999999999998</v>
+      </c>
+      <c r="G2">
+        <f>IF(ISNUMBER('Problem Setup'!H47),ROUND('Problem Setup'!H47,3),"")</f>
+        <v>3.028</v>
+      </c>
+      <c r="H2">
+        <f>IF(ISNUMBER('Problem Setup'!I47),ROUND('Problem Setup'!I47,3),"")</f>
+        <v>1.361</v>
+      </c>
+      <c r="I2">
+        <f>IF(ISNUMBER('Problem Setup'!J47),ROUND('Problem Setup'!J47,3),"")</f>
+        <v>0.61099999999999999</v>
       </c>
       <c r="J2" t="str">
         <f>IF(ISNUMBER('Problem Setup'!K47),'Problem Setup'!K47,"")</f>
@@ -8799,39 +8801,39 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>IF(ISNUMBER('Problem Setup'!B48),'Problem Setup'!B48,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!B48),ROUND('Problem Setup'!B48,3),"")</f>
         <v>0</v>
       </c>
       <c r="B3">
-        <f>IF(ISNUMBER('Problem Setup'!C48),'Problem Setup'!C48,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!C48),ROUND('Problem Setup'!C48,3),"")</f>
         <v>3000</v>
       </c>
       <c r="C3">
-        <f>IF(ISNUMBER('Problem Setup'!D48),'Problem Setup'!D48,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!D48),ROUND('Problem Setup'!D48,3),"")</f>
         <v>7500</v>
       </c>
       <c r="D3">
-        <f>IF(ISNUMBER('Problem Setup'!E48),'Problem Setup'!E48,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!E48),ROUND('Problem Setup'!E48,3),"")</f>
         <v>12500</v>
       </c>
       <c r="E3">
-        <f>IF(ISNUMBER('Problem Setup'!F48),'Problem Setup'!F48,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!F48),ROUND('Problem Setup'!F48,3),"")</f>
         <v>20000</v>
       </c>
       <c r="F3">
-        <f>IF(ISNUMBER('Problem Setup'!G48),'Problem Setup'!G48,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!G48),ROUND('Problem Setup'!G48,3),"")</f>
         <v>30000</v>
       </c>
       <c r="G3" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!H48),'Problem Setup'!H48,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!H48),ROUND('Problem Setup'!H48,3),"")</f>
         <v/>
       </c>
       <c r="H3" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!I48),'Problem Setup'!I48,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!I48),ROUND('Problem Setup'!I48,3),"")</f>
         <v/>
       </c>
       <c r="I3" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!J48),'Problem Setup'!J48,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!J48),ROUND('Problem Setup'!J48,3),"")</f>
         <v/>
       </c>
       <c r="J3" t="str">
@@ -8841,39 +8843,39 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>IF(ISNUMBER('Problem Setup'!B49),'Problem Setup'!B49,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!B49),ROUND('Problem Setup'!B49,3),"")</f>
         <v>10</v>
       </c>
-      <c r="B4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!C49),'Problem Setup'!C49,"")</f>
-        <v>8.6070797642505781</v>
-      </c>
-      <c r="C4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!D49),'Problem Setup'!D49,"")</f>
-        <v>6.8728927879097226</v>
-      </c>
-      <c r="D4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!E49),'Problem Setup'!E49,"")</f>
-        <v>5.3526142851899028</v>
-      </c>
-      <c r="E4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!F49),'Problem Setup'!F49,"")</f>
-        <v>3.6787944117144233</v>
-      </c>
-      <c r="F4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!G49),'Problem Setup'!G49,"")</f>
-        <v>2.2313016014842981</v>
+      <c r="B4">
+        <f>IF(ISNUMBER('Problem Setup'!C49),ROUND('Problem Setup'!C49,3),"")</f>
+        <v>8.6069999999999993</v>
+      </c>
+      <c r="C4">
+        <f>IF(ISNUMBER('Problem Setup'!D49),ROUND('Problem Setup'!D49,3),"")</f>
+        <v>6.8730000000000002</v>
+      </c>
+      <c r="D4">
+        <f>IF(ISNUMBER('Problem Setup'!E49),ROUND('Problem Setup'!E49,3),"")</f>
+        <v>5.3529999999999998</v>
+      </c>
+      <c r="E4">
+        <f>IF(ISNUMBER('Problem Setup'!F49),ROUND('Problem Setup'!F49,3),"")</f>
+        <v>3.6789999999999998</v>
+      </c>
+      <c r="F4">
+        <f>IF(ISNUMBER('Problem Setup'!G49),ROUND('Problem Setup'!G49,3),"")</f>
+        <v>2.2309999999999999</v>
       </c>
       <c r="G4" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!H49),'Problem Setup'!H49,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!H49),ROUND('Problem Setup'!H49,3),"")</f>
         <v/>
       </c>
       <c r="H4" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!I49),'Problem Setup'!I49,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!I49),ROUND('Problem Setup'!I49,3),"")</f>
         <v/>
       </c>
       <c r="I4" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!J49),'Problem Setup'!J49,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!J49),ROUND('Problem Setup'!J49,3),"")</f>
         <v/>
       </c>
       <c r="J4" t="str">
@@ -8883,39 +8885,39 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>IF(ISNUMBER('Problem Setup'!B50),'Problem Setup'!B50,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!B50),ROUND('Problem Setup'!B50,3),"")</f>
         <v>0</v>
       </c>
       <c r="B5">
-        <f>IF(ISNUMBER('Problem Setup'!C50),'Problem Setup'!C50,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!C50),ROUND('Problem Setup'!C50,3),"")</f>
         <v>2500</v>
       </c>
       <c r="C5">
-        <f>IF(ISNUMBER('Problem Setup'!D50),'Problem Setup'!D50,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!D50),ROUND('Problem Setup'!D50,3),"")</f>
         <v>5000</v>
       </c>
       <c r="D5">
-        <f>IF(ISNUMBER('Problem Setup'!E50),'Problem Setup'!E50,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!E50),ROUND('Problem Setup'!E50,3),"")</f>
         <v>10000</v>
       </c>
       <c r="E5">
-        <f>IF(ISNUMBER('Problem Setup'!F50),'Problem Setup'!F50,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!F50),ROUND('Problem Setup'!F50,3),"")</f>
         <v>15000</v>
       </c>
       <c r="F5">
-        <f>IF(ISNUMBER('Problem Setup'!G50),'Problem Setup'!G50,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!G50),ROUND('Problem Setup'!G50,3),"")</f>
         <v>25000</v>
       </c>
       <c r="G5">
-        <f>IF(ISNUMBER('Problem Setup'!H50),'Problem Setup'!H50,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!H50),ROUND('Problem Setup'!H50,3),"")</f>
         <v>35000</v>
       </c>
       <c r="H5" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!I50),'Problem Setup'!I50,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!I50),ROUND('Problem Setup'!I50,3),"")</f>
         <v/>
       </c>
       <c r="I5" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!J50),'Problem Setup'!J50,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!J50),ROUND('Problem Setup'!J50,3),"")</f>
         <v/>
       </c>
       <c r="J5" t="str">
@@ -8925,44 +8927,242 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>IF(ISNUMBER('Problem Setup'!B51),'Problem Setup'!B51,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!B51),ROUND('Problem Setup'!B51,3),"")</f>
         <v>25</v>
       </c>
-      <c r="B6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!C51),'Problem Setup'!C51,"")</f>
-        <v>19.470019576785123</v>
-      </c>
-      <c r="C6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!D51),'Problem Setup'!D51,"")</f>
-        <v>15.163266492815836</v>
-      </c>
-      <c r="D6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!E51),'Problem Setup'!E51,"")</f>
-        <v>9.1969860292860588</v>
-      </c>
-      <c r="E6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!F51),'Problem Setup'!F51,"")</f>
-        <v>5.5782540037107458</v>
-      </c>
-      <c r="F6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!G51),'Problem Setup'!G51,"")</f>
-        <v>2.05212496559747</v>
-      </c>
-      <c r="G6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!H51),'Problem Setup'!H51,"")</f>
-        <v>0.75493458555796256</v>
+      <c r="B6">
+        <f>IF(ISNUMBER('Problem Setup'!C51),ROUND('Problem Setup'!C51,3),"")</f>
+        <v>19.47</v>
+      </c>
+      <c r="C6">
+        <f>IF(ISNUMBER('Problem Setup'!D51),ROUND('Problem Setup'!D51,3),"")</f>
+        <v>15.163</v>
+      </c>
+      <c r="D6">
+        <f>IF(ISNUMBER('Problem Setup'!E51),ROUND('Problem Setup'!E51,3),"")</f>
+        <v>9.1969999999999992</v>
+      </c>
+      <c r="E6">
+        <f>IF(ISNUMBER('Problem Setup'!F51),ROUND('Problem Setup'!F51,3),"")</f>
+        <v>5.5780000000000003</v>
+      </c>
+      <c r="F6">
+        <f>IF(ISNUMBER('Problem Setup'!G51),ROUND('Problem Setup'!G51,3),"")</f>
+        <v>2.052</v>
+      </c>
+      <c r="G6">
+        <f>IF(ISNUMBER('Problem Setup'!H51),ROUND('Problem Setup'!H51,3),"")</f>
+        <v>0.755</v>
       </c>
       <c r="H6" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!I51),'Problem Setup'!I51,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!I51),ROUND('Problem Setup'!I51,3),"")</f>
         <v/>
       </c>
       <c r="I6" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!J51),'Problem Setup'!J51,"")</f>
+        <f>IF(ISNUMBER('Problem Setup'!J51),ROUND('Problem Setup'!J51,3),"")</f>
         <v/>
       </c>
       <c r="J6" t="str">
         <f>IF(ISNUMBER('Problem Setup'!K51),'Problem Setup'!K51,"")</f>
         <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.75</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.25</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1.25</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1.3</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.3</v>
       </c>
     </row>
   </sheetData>
@@ -8970,264 +9170,335 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+      <c r="D1">
+        <v>5000</v>
+      </c>
+      <c r="E1">
+        <v>10000</v>
+      </c>
+      <c r="F1">
+        <v>15000</v>
+      </c>
+      <c r="G1">
+        <v>20000</v>
+      </c>
+      <c r="H1">
+        <v>30000</v>
+      </c>
+      <c r="I1">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>2661</v>
+      </c>
+      <c r="E2" s="7">
+        <v>8147</v>
+      </c>
+      <c r="F2" s="7">
+        <v>13753</v>
+      </c>
+      <c r="G2" s="7">
+        <v>19134</v>
+      </c>
+      <c r="H2" s="7">
+        <v>29426</v>
+      </c>
+      <c r="I2" s="7">
+        <v>39487</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2500</v>
+      </c>
+      <c r="E3">
+        <v>5000</v>
+      </c>
+      <c r="F3">
+        <v>10000</v>
+      </c>
+      <c r="G3">
+        <v>15000</v>
+      </c>
+      <c r="H3">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1390</v>
+      </c>
+      <c r="F4" s="7">
+        <v>6275</v>
+      </c>
+      <c r="G4" s="7">
+        <v>11866</v>
+      </c>
+      <c r="H4" s="7">
+        <v>17515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="E5">
+        <v>10000</v>
+      </c>
+      <c r="F5">
+        <v>17500</v>
+      </c>
+      <c r="G5">
+        <v>25000</v>
+      </c>
+      <c r="H5">
+        <v>35000</v>
+      </c>
+      <c r="I5">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1467</v>
+      </c>
+      <c r="E6" s="7">
+        <v>5821</v>
+      </c>
+      <c r="F6" s="7">
+        <v>13959</v>
+      </c>
+      <c r="G6" s="7">
+        <v>22448</v>
+      </c>
+      <c r="H6" s="7">
+        <v>33443</v>
+      </c>
+      <c r="I6" s="7">
+        <v>41917</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2500</v>
+      </c>
+      <c r="E11">
+        <v>5000</v>
+      </c>
+      <c r="F11">
+        <v>7500</v>
+      </c>
+      <c r="G11">
+        <v>10000</v>
+      </c>
+      <c r="H11">
+        <v>15000</v>
+      </c>
+      <c r="I11">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" s="6">
+        <v>303</v>
+      </c>
+      <c r="E12">
+        <v>1717</v>
+      </c>
+      <c r="F12">
+        <v>3707</v>
+      </c>
+      <c r="G12">
+        <v>6071</v>
+      </c>
+      <c r="H12">
+        <v>11403</v>
+      </c>
+      <c r="I12">
+        <v>14209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <f>IF(ISNUMBER('Problem Setup'!B46),'Problem Setup'!B46,"")</f>
+        <v>10050.640386179501</v>
+      </c>
+      <c r="B1">
+        <v>11312.9692076274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>22028.156015179</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B1">
-        <f>IF(ISNUMBER('Problem Setup'!C46),'Problem Setup'!C46,"")</f>
-        <v>2000</v>
-      </c>
-      <c r="C1">
-        <f>IF(ISNUMBER('Problem Setup'!D46),'Problem Setup'!D46,"")</f>
-        <v>4000</v>
-      </c>
-      <c r="D1">
-        <f>IF(ISNUMBER('Problem Setup'!E46),'Problem Setup'!E46,"")</f>
-        <v>7500</v>
-      </c>
-      <c r="E1">
-        <f>IF(ISNUMBER('Problem Setup'!F46),'Problem Setup'!F46,"")</f>
-        <v>10000</v>
-      </c>
-      <c r="F1">
-        <f>IF(ISNUMBER('Problem Setup'!G46),'Problem Setup'!G46,"")</f>
-        <v>15000</v>
-      </c>
-      <c r="G1">
-        <f>IF(ISNUMBER('Problem Setup'!H46),'Problem Setup'!H46,"")</f>
-        <v>20000</v>
-      </c>
-      <c r="H1">
-        <f>IF(ISNUMBER('Problem Setup'!I46),'Problem Setup'!I46,"")</f>
-        <v>30000</v>
-      </c>
-      <c r="I1">
-        <f>IF(ISNUMBER('Problem Setup'!J46),'Problem Setup'!J46,"")</f>
-        <v>40000</v>
-      </c>
-      <c r="J1" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!K46),'Problem Setup'!K46,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>IF(ISNUMBER('Problem Setup'!B47),'Problem Setup'!B47,"")</f>
-        <v>15</v>
-      </c>
-      <c r="B2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!C47),'Problem Setup'!C47,"")</f>
-        <v>12.78215683449317</v>
-      </c>
-      <c r="C2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!D47),'Problem Setup'!D47,"")</f>
-        <v>10.892235556105364</v>
-      </c>
-      <c r="D2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!E47),'Problem Setup'!E47,"")</f>
-        <v>8.2321745414103962</v>
-      </c>
-      <c r="E2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!F47),'Problem Setup'!F47,"")</f>
-        <v>6.7399344617583239</v>
-      </c>
-      <c r="F2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!G47),'Problem Setup'!G47,"")</f>
-        <v>4.5179131786830302</v>
-      </c>
-      <c r="G2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!H47),'Problem Setup'!H47,"")</f>
-        <v>3.0284477699198309</v>
-      </c>
-      <c r="H2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!I47),'Problem Setup'!I47,"")</f>
-        <v>1.3607692993411871</v>
-      </c>
-      <c r="I2" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!J47),'Problem Setup'!J47,"")</f>
-        <v>0.61143305967549322</v>
-      </c>
-      <c r="J2" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!K47),'Problem Setup'!K47,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>IF(ISNUMBER('Problem Setup'!B48),'Problem Setup'!B48,"")</f>
         <v>0</v>
       </c>
       <c r="B3">
-        <f>IF(ISNUMBER('Problem Setup'!C48),'Problem Setup'!C48,"")</f>
-        <v>3000</v>
-      </c>
-      <c r="C3">
-        <f>IF(ISNUMBER('Problem Setup'!D48),'Problem Setup'!D48,"")</f>
-        <v>7500</v>
-      </c>
-      <c r="D3">
-        <f>IF(ISNUMBER('Problem Setup'!E48),'Problem Setup'!E48,"")</f>
-        <v>12500</v>
-      </c>
-      <c r="E3">
-        <f>IF(ISNUMBER('Problem Setup'!F48),'Problem Setup'!F48,"")</f>
-        <v>20000</v>
-      </c>
-      <c r="F3">
-        <f>IF(ISNUMBER('Problem Setup'!G48),'Problem Setup'!G48,"")</f>
-        <v>30000</v>
-      </c>
-      <c r="G3" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!H48),'Problem Setup'!H48,"")</f>
-        <v/>
-      </c>
-      <c r="H3" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!I48),'Problem Setup'!I48,"")</f>
-        <v/>
-      </c>
-      <c r="I3" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!J48),'Problem Setup'!J48,"")</f>
-        <v/>
-      </c>
-      <c r="J3" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!K48),'Problem Setup'!K48,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <f>IF(ISNUMBER('Problem Setup'!B49),'Problem Setup'!B49,"")</f>
-        <v>10</v>
-      </c>
-      <c r="B4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!C49),'Problem Setup'!C49,"")</f>
-        <v>8.6070797642505781</v>
-      </c>
-      <c r="C4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!D49),'Problem Setup'!D49,"")</f>
-        <v>6.8728927879097226</v>
-      </c>
-      <c r="D4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!E49),'Problem Setup'!E49,"")</f>
-        <v>5.3526142851899028</v>
-      </c>
-      <c r="E4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!F49),'Problem Setup'!F49,"")</f>
-        <v>3.6787944117144233</v>
-      </c>
-      <c r="F4" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!G49),'Problem Setup'!G49,"")</f>
-        <v>2.2313016014842981</v>
-      </c>
-      <c r="G4" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!H49),'Problem Setup'!H49,"")</f>
-        <v/>
-      </c>
-      <c r="H4" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!I49),'Problem Setup'!I49,"")</f>
-        <v/>
-      </c>
-      <c r="I4" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!J49),'Problem Setup'!J49,"")</f>
-        <v/>
-      </c>
-      <c r="J4" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!K49),'Problem Setup'!K49,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f>IF(ISNUMBER('Problem Setup'!B50),'Problem Setup'!B50,"")</f>
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <f>IF(ISNUMBER('Problem Setup'!C50),'Problem Setup'!C50,"")</f>
-        <v>2500</v>
-      </c>
-      <c r="C5">
-        <f>IF(ISNUMBER('Problem Setup'!D50),'Problem Setup'!D50,"")</f>
-        <v>5000</v>
-      </c>
-      <c r="D5">
-        <f>IF(ISNUMBER('Problem Setup'!E50),'Problem Setup'!E50,"")</f>
-        <v>10000</v>
-      </c>
-      <c r="E5">
-        <f>IF(ISNUMBER('Problem Setup'!F50),'Problem Setup'!F50,"")</f>
-        <v>15000</v>
-      </c>
-      <c r="F5">
-        <f>IF(ISNUMBER('Problem Setup'!G50),'Problem Setup'!G50,"")</f>
-        <v>25000</v>
-      </c>
-      <c r="G5">
-        <f>IF(ISNUMBER('Problem Setup'!H50),'Problem Setup'!H50,"")</f>
-        <v>35000</v>
-      </c>
-      <c r="H5" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!I50),'Problem Setup'!I50,"")</f>
-        <v/>
-      </c>
-      <c r="I5" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!J50),'Problem Setup'!J50,"")</f>
-        <v/>
-      </c>
-      <c r="J5" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!K50),'Problem Setup'!K50,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>IF(ISNUMBER('Problem Setup'!B51),'Problem Setup'!B51,"")</f>
-        <v>25</v>
-      </c>
-      <c r="B6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!C51),'Problem Setup'!C51,"")</f>
-        <v>19.470019576785123</v>
-      </c>
-      <c r="C6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!D51),'Problem Setup'!D51,"")</f>
-        <v>15.163266492815836</v>
-      </c>
-      <c r="D6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!E51),'Problem Setup'!E51,"")</f>
-        <v>9.1969860292860588</v>
-      </c>
-      <c r="E6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!F51),'Problem Setup'!F51,"")</f>
-        <v>5.5782540037107458</v>
-      </c>
-      <c r="F6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!G51),'Problem Setup'!G51,"")</f>
-        <v>2.05212496559747</v>
-      </c>
-      <c r="G6" s="6">
-        <f>IF(ISNUMBER('Problem Setup'!H51),'Problem Setup'!H51,"")</f>
-        <v>0.75493458555796256</v>
-      </c>
-      <c r="H6" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!I51),'Problem Setup'!I51,"")</f>
-        <v/>
-      </c>
-      <c r="I6" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!J51),'Problem Setup'!J51,"")</f>
-        <v/>
-      </c>
-      <c r="J6" t="str">
-        <f>IF(ISNUMBER('Problem Setup'!K51),'Problem Setup'!K51,"")</f>
-        <v/>
+        <v>13684.530792372499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>